<commit_message>
Update Project06 - 요구사항 정의서 초안.xlsx
</commit_message>
<xml_diff>
--- a/2. 기능정리 취합/Project06 - 요구사항 정의서 초안.xlsx
+++ b/2. 기능정리 취합/Project06 - 요구사항 정의서 초안.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\project06\2. 기능정리 취합\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HYEONTAE\Desktop\project06\2. 기능정리 취합\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49C2EAB1-83F2-4B92-9504-9645BD8AAE5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항정의서" sheetId="1" r:id="rId1"/>
     <sheet name="조원 역할 분배" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항정의서!$A$7:$P$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">요구사항정의서!$A$7:$P$50</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="167">
   <si>
     <t>현태</t>
   </si>
@@ -227,12 +226,6 @@
     <t>HT – M - 010</t>
   </si>
   <si>
-    <t>KB – P – 013</t>
-  </si>
-  <si>
-    <t>KB – M – 013</t>
-  </si>
-  <si>
     <t>YS – P – 014
 YS – P – 015</t>
   </si>
@@ -257,349 +250,516 @@
   </si>
   <si>
     <t>사용자</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>관리자</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>메인페이지</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원등록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 상세보기</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심 프로젝트 등록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>펀딩하기</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 신고</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 정보확인(메이커명, 목표금액, 기간, 정산방법 등)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 상세보기</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 구매</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리별 상품 목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이페이지</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원정보변경</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원탈퇴</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의 계좌</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로필 수정 페이지 내 회원탈퇴 버튼을 통해 탈퇴 가능</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>메이커 스튜디오</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>메이커 등록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 등록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트를 오픈할 수 있는 메이커 회원(기업) 등록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지사항</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAQ</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 문의</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트에 대한 문의, 메이커의 답변 확인</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 문의</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품에 대한 문의, 메이커의 답변 확인</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>이슈 및 사이트 공지사항</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회사 메인 컨셉 소개 및 펀딩 참여, 펀딩 오픈, 사이트 이용 방법 등 자주 묻는 질문</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객센터 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 상세보기</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 승인</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 수정</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 정산</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>간단한 정보관리 및 불량회원에 대한 제제(투자제한)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>오픈 신청한 프로젝트의 정보 확인 후 승인 또는 거절</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>오픈 승인된 프로젝트의 문제 발생 시 수정</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매중인 상품 문제 발생 시 수정</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>로그인/로그아웃, 회원가입, 알림
-프로젝트 검색, 카테고리별 프로젝트 리스트, 슬라이드 배너광고, 추천 프로젝트 리스트, 마감 직전 프로젝트, 펀딩 성공 프로젝트, 리워드 펀딩 성공 판매상품</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원등록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디, 비밀번호 입력 로그인
+프로젝트 검색, 카테고리별 프로젝트 리스트 네비게이션 바, 슬라이드 배너광고, 추천 프로젝트 리스트(관리자가 선택한 프로젝트), 마감 직전 프로젝트, 리워드 펀딩 성공 판매 상품</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일, 비밀번호 입력 로그인
 네이버, 카카오톡, 구글 간편로그인</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디/비밀번호 찾기</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일 찾기/비밀번호 찾기</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>네이버, 카카오톡, 구글 간편 회원가입
-아이디 중복확인, 비밀번호 재입력, 이름, 전화번호,이메일 등의 개인정보 입력 후 가입
-관심카테고리 설정
-## 이메일 주소, 이름, 비밀번호만으로 회원가입  간편 회원가입</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>가입 시 이용한 이름, 이메일을 통해서 아이디 찾기
-가입 시 이용한 이름, 이메일, 아이디, 휴대폰번호를 이용하여 비밀번호 찾기</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+## 이메일 주소, 이름, 비밀번호만으로 회원가입, 관심카테고리 설정  간편 회원가입
+상세정보(전화번호, 계좌) - 필요한 서비스를 이용할때 등록이 안되어있다면 추가하라는 알림이 뜸</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>이메일 찾기 - 이메일을 입력해보세요 서비스 가입 여부를 확인해드립니다 or 휴대폰번호를 입력해보세요
+비밀번호 찾기 - 가입 시 이용한 이름, 이메일 or 휴대폰번호를 이용하여 이메일로 임시비밀번호 전송</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>펀딩</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 목록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 상세보기</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>관심 프로젝트 등록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>펀딩하기</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 신고</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>투자 / 리워드, 카테고리별 프로젝트 목록, 오픈예정 프로젝트, 성공 및 달성 가능성 높은 프로젝트 목록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 정보확인(메이커명, 목표금액, 기간, 정산방법 등)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>리워드 판매 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>리워드 상품 옵션, 주문 확인, 배송 설정</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>투자 / 리워드, 카테고리별 프로젝트 목록, 오픈예정 프로젝트, 달성 완료 프로젝트, 달성 실패 프로젝트, 성공 및 달성 가능성 높은 프로젝트 목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 기본정보(프로젝트명, 카테고리, 진행기간(시작 날짜, 종료 날짜), 목표금액, 가격, 이미지 등)
+프로젝트 정산방법 및 세부내용 작성 후 등록 신청
+관리자 승인 후 오픈가능</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>상세 페이지에서 관심 프로젝트 등록, 마이페이지에서 확인 가능</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>투자프로젝트인 경우 금액 선택 후 결제
-리워드프로젝트인 경우 옵션에 따른 상품 및 금액 선택 후 배송정보 입력, 결제</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>불량 프로젝트 신고 페이지로 이동, 신고 시 증거자료 제출 필요</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>리워드 샵</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 목록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 상세보기</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 구매</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>카테고리별 상품 목록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 정보(메이커명, 상품명, 상세정보 등)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>구매 정보, 배송지, 결제정보 입력 후 결제</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>마이페이지</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원정보변경</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원탈퇴</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>나의 계좌</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+리워드프로젝트인 경우 옵션에 따른 상품 및 금액 선택 후 배송정보 입력, 결제 - 등록한 배송지를 기본 배송지로 설정하시겠습니까?</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>불량 프로젝트 신고 페이지로 이동, 신고 시 증거자료 제출 필요(파일 업로드)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 정보(메이커명, 상품명, 상세정보(가격, 이미지-프로젝트 관련 내용 포함, 상세 내용 등))</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입시 입력한 정보를 수정, 관심 카테고리 설정</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>나의 펀딩</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심 프로젝트</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심 프로젝트 목록 및 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>주문조회</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입시 입력한 정보를 수정, 관심 카테고리 설정</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로필 수정 페이지 내 회원탈퇴 버튼을 통해 탈퇴 가능</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>수익금 정산 받을 계좌 등록 및 수정, 예치금 충전 및 이용내역</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>펀딩한 프로젝트의 목록, 진행상태 확인
-관심 프로젝트 목록 및 관리</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>리워드 스토어</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>리워드 샵에서 구매한 상품의 주문/배송 조회</t>
-  </si>
-  <si>
-    <t>메이커 스튜디오</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>메이커 등록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 등록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 관리</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트를 오픈할 수 있는 메이커 회원(기업) 등록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 기본정보(프로젝트명, 카테고리, 진행기간, 목표금액 또는 목표수량, 가격, 이미지 등)
-프로젝트 정산방법 및 세부내용 작성
-관리자 승인 후 오픈가능</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객센터</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>메이커 목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>메이커 목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 조회 및 상세 내용 확인 및 회원 상태(정상, 제제, 제명) 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>메이커 조회 및 상세 내용 확인 및 메이커 상태(정상, 제제, 제명) 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 계정 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>마스터 관리자 계정
+관리자 계정 등록, 수정
+마스터 관리자는 관리자 권한 부여 기능</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>진행 이전 프로젝트
+진행 중 프로젝트
+진행 완료 프로젝트</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>펀딩한 프로젝트의 목록, 진행상태 확인</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매 정보(개수 선택), 배송지, 결제정보 입력 후 결제</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>정산 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">완료 된 프로젝트의 정산 상태 확인 (최종 펀딩 받은 금액, 정산 진행 상태(정산전, x회차 정산 중, 정산완료)) </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트별 / 회차별 입금 해야 하는 금액 및 기간</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>스토어 등록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>리워드 스토어 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>신청된 상품들과 판매되는 상품 목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>펀딩 성공한 리워드 프로젝트에 한하여 오픈신청 및 관리자 승인 후 오픈
+상품정보(상품명, 상품 상세설명), 가격 등 설정 후 등록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAQ</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">공지사항 </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAQ 목록, FAQ 등록 및 수정</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지사항 목록, 공지사항 등록 및 수정</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>리워드 스토어 승인</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>리워드 스토어 수정</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>리워드 스토어 목록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>신청 받은 펀딩 성공 리워드 상품에 대한 스토어 오픈 정보 및 상품 옵션 검토 후 승인 또는 거절</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원들의 1:1문의와 채팅 문의 답변 작성</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>오픈한 프로젝트 목록 및 상세정보
-승인된 프로젝트 오픈 전 수정</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>펀딩 성공한 리워드 프로젝트에 한하여 오픈신청
-상품정보, 가격 등 수정 후 등록
-상품 판매 관리</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>고객센터</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>공지사항</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>FAQ</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>1:1 문의</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+승인된 프로젝트 오픈 전 수정
+문의 사항 답변</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>문의 글 등록하면 관리자가 답변을 해주는 형태, 바로 답변이 진행이 되면 채팅 형식으로 진행, 바로 답변이 안되면 시간이 지난 후 확인 가능 하도록</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>실시간 채팅 상담</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 문의</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트에 대한 문의, 메이커의 답변 확인</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 문의</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품에 대한 문의, 메이커의 답변 확인</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>이슈 및 사이트 공지사항</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회사 메인 컨셉 소개 및 펀딩 참여, 펀딩 오픈, 사이트 이용 방법 등 자주 묻는 질문</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>서비스 이용에 대한 문의, 관리자의 답변 확인</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>실시간 채팅을 통한 문의 응대 및 답변</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원관리</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>리워드 샵 관리</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>고객센터 관리</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원목록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 상세보기</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 승인</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 수정</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 정산</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 조회</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 승인</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>상품 수정</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 목록, 일반 서포터 회원 / 메이커 회원 구분에 따른 조회</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>간단한 정보관리 및 불량회원에 대한 제제(투자제한)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>오픈 신청한 프로젝트부터 종료된 프로젝트까지의 목록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>오픈 신청한 프로젝트의 정보 확인 후 승인 또는 거절</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>오픈 승인된 프로젝트의 문제 발생 시 수정</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>신청된 상품들과 판매되는 상품 목록</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>신청 받은 펀딩 성공 리워드 상품에 대한 스토어 오픈 정보 검토 후 승인 또는 거절</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>판매중인 상품 문제 발생 시 수정</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>공지사항목록, 공지사항 등록 및 수정</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원들의 1:1문의 목록, 1:1문의에 대한 답변 작성</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>실시간 채팅 상담 관리</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>형준</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>현태</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>현태</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>현태</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>민기</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>민기</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>기범</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>기범</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>기범</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>서희</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>서희</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>송우</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>송우</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>형준</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>형준</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>형준</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>형준</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>형준</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>송우</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>송우</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>송우</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>기범</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>기범</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>수익금 정산 받을 계좌 등록 및 수정, 예치금 충전 및 이용내역, 출금</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>형준</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>현태</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -658,11 +818,6 @@
       <charset val="129"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
@@ -696,6 +851,13 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -723,7 +885,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -992,19 +1154,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1084,11 +1278,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1103,89 +1360,59 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1401,10 +1628,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG1009"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -1463,22 +1690,22 @@
     </row>
     <row r="2" spans="1:33" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="52"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -1500,20 +1727,20 @@
     </row>
     <row r="3" spans="1:33" ht="19.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="55"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -1661,13 +1888,13 @@
       <c r="F7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="37"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="58"/>
       <c r="L7" s="5" t="s">
         <v>19</v>
       </c>
@@ -1747,18 +1974,20 @@
       <c r="AG8" s="1"/>
     </row>
     <row r="9" spans="1:33" ht="46.95" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48" t="s">
-        <v>49</v>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34" t="s">
+        <v>89</v>
       </c>
       <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="21" t="s">
+        <v>141</v>
+      </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
@@ -1794,18 +2023,20 @@
       <c r="AG9" s="1"/>
     </row>
     <row r="10" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A10" s="49"/>
-      <c r="B10" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="48" t="s">
-        <v>52</v>
+      <c r="A10" s="43"/>
+      <c r="B10" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>90</v>
       </c>
       <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="F10" s="20" t="s">
+        <v>154</v>
+      </c>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
@@ -1841,16 +2072,18 @@
       <c r="AG10" s="1"/>
     </row>
     <row r="11" spans="1:33" ht="63" customHeight="1">
-      <c r="A11" s="49"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>55</v>
+      <c r="A11" s="43"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>92</v>
       </c>
       <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="F11" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
@@ -1880,16 +2113,18 @@
       <c r="AG11" s="1"/>
     </row>
     <row r="12" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A12" s="49"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="48" t="s">
-        <v>56</v>
+      <c r="A12" s="43"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>93</v>
       </c>
       <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="F12" s="20" t="s">
+        <v>156</v>
+      </c>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
@@ -1919,18 +2154,20 @@
       <c r="AG12" s="1"/>
     </row>
     <row r="13" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A13" s="49"/>
-      <c r="B13" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="48" t="s">
-        <v>63</v>
+      <c r="A13" s="43"/>
+      <c r="B13" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>69</v>
       </c>
       <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="F13" s="20" t="s">
+        <v>142</v>
+      </c>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
@@ -1938,15 +2175,9 @@
       <c r="K13" s="22"/>
       <c r="L13" s="23"/>
       <c r="M13" s="24"/>
-      <c r="N13" s="17">
-        <v>2</v>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="10" t="s">
-        <v>29</v>
-      </c>
+      <c r="N13" s="17"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -1965,17 +2196,19 @@
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A14" s="49"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>64</v>
+    <row r="14" spans="1:33" ht="46.95" customHeight="1">
+      <c r="A14" s="43"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>98</v>
       </c>
       <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="F14" s="20" t="s">
+        <v>142</v>
+      </c>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
@@ -2004,17 +2237,19 @@
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A15" s="49"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>65</v>
+    <row r="15" spans="1:33" ht="46.8">
+      <c r="A15" s="43"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="F15" s="20" t="s">
+        <v>142</v>
+      </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
@@ -2044,32 +2279,28 @@
       <c r="AG15" s="1"/>
     </row>
     <row r="16" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A16" s="49"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>66</v>
+      <c r="A16" s="43"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
+      <c r="F16" s="20" t="s">
+        <v>142</v>
+      </c>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="23"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="17">
-        <v>1</v>
-      </c>
-      <c r="O16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="P16" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="M16" s="24"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -2088,24 +2319,26 @@
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
     </row>
-    <row r="17" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>67</v>
+    <row r="17" spans="1:33" ht="46.95" customHeight="1">
+      <c r="A17" s="43"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>127</v>
       </c>
       <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
+      <c r="F17" s="20" t="s">
+        <v>143</v>
+      </c>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="23"/>
-      <c r="M17" s="25"/>
+      <c r="M17" s="24"/>
       <c r="N17" s="17"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
@@ -2127,17 +2360,19 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A18" s="49"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="63" t="s">
-        <v>100</v>
+    <row r="18" spans="1:33" ht="46.95" customHeight="1">
+      <c r="A18" s="43"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>96</v>
       </c>
       <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
+      <c r="F18" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
@@ -2145,15 +2380,9 @@
       <c r="K18" s="22"/>
       <c r="L18" s="23"/>
       <c r="M18" s="24"/>
-      <c r="N18" s="17">
-        <v>1</v>
-      </c>
-      <c r="O18" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="P18" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="N18" s="17"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -2173,18 +2402,20 @@
       <c r="AG18" s="1"/>
     </row>
     <row r="19" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>72</v>
+      <c r="A19" s="43"/>
+      <c r="B19" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>97</v>
       </c>
       <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
+      <c r="F19" s="20" t="s">
+        <v>145</v>
+      </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
@@ -2192,9 +2423,15 @@
       <c r="K19" s="22"/>
       <c r="L19" s="23"/>
       <c r="M19" s="24"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="N19" s="17">
+        <v>2</v>
+      </c>
+      <c r="O19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -2214,16 +2451,18 @@
       <c r="AG19" s="1"/>
     </row>
     <row r="20" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A20" s="49"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="58" t="s">
-        <v>73</v>
+      <c r="A20" s="43"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>55</v>
       </c>
       <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
+      <c r="F20" s="20" t="s">
+        <v>146</v>
+      </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
@@ -2253,16 +2492,18 @@
       <c r="AG20" s="1"/>
     </row>
     <row r="21" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A21" s="49"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>74</v>
+      <c r="A21" s="43"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>99</v>
       </c>
       <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
+      <c r="F21" s="20" t="s">
+        <v>145</v>
+      </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
@@ -2292,26 +2533,34 @@
       <c r="AG21" s="1"/>
     </row>
     <row r="22" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A22" s="49"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="58" t="s">
-        <v>102</v>
+      <c r="A22" s="43"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>100</v>
       </c>
       <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
+      <c r="F22" s="20" t="s">
+        <v>146</v>
+      </c>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="23"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="17">
+        <v>1</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2331,25 +2580,25 @@
       <c r="AG22" s="1"/>
     </row>
     <row r="23" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A23" s="49"/>
-      <c r="B23" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>81</v>
+      <c r="A23" s="43"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>101</v>
       </c>
       <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
+      <c r="F23" s="20" t="s">
+        <v>145</v>
+      </c>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
       <c r="L23" s="23"/>
-      <c r="M23" s="24"/>
+      <c r="M23" s="25"/>
       <c r="N23" s="17"/>
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
@@ -2372,16 +2621,18 @@
       <c r="AG23" s="1"/>
     </row>
     <row r="24" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A24" s="49"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="48" t="s">
-        <v>82</v>
+      <c r="A24" s="43"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>73</v>
       </c>
       <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="F24" s="20" t="s">
+        <v>146</v>
+      </c>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
@@ -2389,9 +2640,15 @@
       <c r="K24" s="22"/>
       <c r="L24" s="23"/>
       <c r="M24" s="24"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="N24" s="17">
+        <v>1</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2411,16 +2668,20 @@
       <c r="AG24" s="1"/>
     </row>
     <row r="25" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A25" s="49"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="48" t="s">
-        <v>83</v>
+      <c r="A25" s="43"/>
+      <c r="B25" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="F25" s="20" t="s">
+        <v>147</v>
+      </c>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
@@ -2450,16 +2711,18 @@
       <c r="AG25" s="1"/>
     </row>
     <row r="26" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A26" s="49"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>84</v>
+      <c r="A26" s="43"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>102</v>
       </c>
       <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
+      <c r="F26" s="20" t="s">
+        <v>148</v>
+      </c>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
@@ -2489,16 +2752,18 @@
       <c r="AG26" s="1"/>
     </row>
     <row r="27" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A27" s="49"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="48" t="s">
-        <v>85</v>
+      <c r="A27" s="43"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>120</v>
       </c>
       <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
+      <c r="F27" s="20" t="s">
+        <v>147</v>
+      </c>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
@@ -2528,18 +2793,18 @@
       <c r="AG27" s="1"/>
     </row>
     <row r="28" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A28" s="49"/>
-      <c r="B28" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="63" t="s">
-        <v>90</v>
+      <c r="A28" s="43"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>75</v>
       </c>
       <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="F28" s="20" t="s">
+        <v>149</v>
+      </c>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
@@ -2568,17 +2833,21 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row r="29" spans="1:33" ht="46.95" customHeight="1">
-      <c r="A29" s="49"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="57" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="48" t="s">
-        <v>91</v>
+    <row r="29" spans="1:33" ht="28.95" customHeight="1">
+      <c r="A29" s="43"/>
+      <c r="B29" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>103</v>
       </c>
       <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+      <c r="F29" s="20" t="s">
+        <v>150</v>
+      </c>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
@@ -2608,16 +2877,18 @@
       <c r="AG29" s="1"/>
     </row>
     <row r="30" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A30" s="49"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="57" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="48" t="s">
-        <v>92</v>
+      <c r="A30" s="43"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
+      <c r="F30" s="20" t="s">
+        <v>150</v>
+      </c>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
@@ -2646,17 +2917,19 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
     </row>
-    <row r="31" spans="1:33" ht="46.95" customHeight="1">
-      <c r="A31" s="49"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="57" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="48" t="s">
-        <v>93</v>
+    <row r="31" spans="1:33" ht="28.95" customHeight="1">
+      <c r="A31" s="43"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>164</v>
       </c>
       <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+      <c r="F31" s="20" t="s">
+        <v>151</v>
+      </c>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
@@ -2686,34 +2959,28 @@
       <c r="AG31" s="1"/>
     </row>
     <row r="32" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A32" s="49"/>
-      <c r="B32" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="60" t="s">
-        <v>103</v>
+      <c r="A32" s="43"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>119</v>
       </c>
       <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
+      <c r="F32" s="20" t="s">
+        <v>150</v>
+      </c>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
-      <c r="I32" s="26"/>
+      <c r="I32" s="22"/>
       <c r="J32" s="22"/>
       <c r="K32" s="22"/>
       <c r="L32" s="23"/>
       <c r="M32" s="24"/>
-      <c r="N32" s="17">
-        <v>2</v>
-      </c>
-      <c r="O32" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="P32" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="N32" s="17"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -2733,32 +3000,28 @@
       <c r="AG32" s="1"/>
     </row>
     <row r="33" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A33" s="49"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" s="60" t="s">
-        <v>104</v>
+      <c r="A33" s="43"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>106</v>
       </c>
       <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
+      <c r="F33" s="20" t="s">
+        <v>150</v>
+      </c>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
-      <c r="I33" s="26"/>
+      <c r="I33" s="22"/>
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
       <c r="L33" s="23"/>
       <c r="M33" s="24"/>
-      <c r="N33" s="17">
-        <v>1</v>
-      </c>
-      <c r="O33" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="P33" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="N33" s="17"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -2778,19 +3041,21 @@
       <c r="AG33" s="1"/>
     </row>
     <row r="34" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A34" s="49"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="59" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="61" t="s">
-        <v>105</v>
+      <c r="A34" s="43"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>109</v>
       </c>
       <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
+      <c r="F34" s="20" t="s">
+        <v>150</v>
+      </c>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
-      <c r="I34" s="26"/>
+      <c r="I34" s="22"/>
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
       <c r="L34" s="23"/>
@@ -2817,16 +3082,20 @@
       <c r="AG34" s="1"/>
     </row>
     <row r="35" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A35" s="62"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="D35" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="24"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20" t="s">
+        <v>152</v>
+      </c>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
@@ -2834,15 +3103,9 @@
       <c r="K35" s="22"/>
       <c r="L35" s="23"/>
       <c r="M35" s="24"/>
-      <c r="N35" s="17">
-        <v>1</v>
-      </c>
-      <c r="O35" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="P35" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="N35" s="17"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -2862,32 +3125,34 @@
       <c r="AG35" s="1"/>
     </row>
     <row r="36" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A36" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" s="26"/>
-      <c r="F36" s="27"/>
+      <c r="A36" s="43"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20" t="s">
+        <v>153</v>
+      </c>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
+      <c r="I36" s="26"/>
       <c r="J36" s="22"/>
       <c r="K36" s="22"/>
       <c r="L36" s="23"/>
       <c r="M36" s="24"/>
       <c r="N36" s="17">
-        <v>3</v>
-      </c>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P36" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -2906,32 +3171,34 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
     </row>
-    <row r="37" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A37" s="39"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="64" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="25"/>
+    <row r="37" spans="1:33" ht="28.95" customHeight="1" thickBot="1">
+      <c r="A37" s="67"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="74"/>
       <c r="N37" s="17">
         <v>1</v>
       </c>
-      <c r="O37" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="P37" s="11" t="s">
-        <v>41</v>
+      <c r="O37" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P37" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -2952,28 +3219,34 @@
       <c r="AG37" s="1"/>
     </row>
     <row r="38" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A38" s="39"/>
-      <c r="B38" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
+      <c r="A38" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="63"/>
+      <c r="F38" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="64"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="17">
+        <v>3</v>
+      </c>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
@@ -2993,26 +3266,34 @@
       <c r="AG38" s="1"/>
     </row>
     <row r="39" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A39" s="39"/>
-      <c r="B39" s="39"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="61"/>
       <c r="C39" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>121</v>
+        <v>81</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>85</v>
       </c>
       <c r="E39" s="26"/>
-      <c r="F39" s="24"/>
+      <c r="F39" s="24" t="s">
+        <v>154</v>
+      </c>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
-      <c r="L39" s="28"/>
+      <c r="L39" s="27"/>
       <c r="M39" s="25"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
+      <c r="N39" s="17">
+        <v>1</v>
+      </c>
+      <c r="O39" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="P39" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
@@ -3032,22 +3313,26 @@
       <c r="AG39" s="1"/>
     </row>
     <row r="40" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A40" s="39"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>122</v>
+      <c r="A40" s="61"/>
+      <c r="B40" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>114</v>
       </c>
       <c r="E40" s="26"/>
-      <c r="F40" s="24"/>
+      <c r="F40" s="24" t="s">
+        <v>158</v>
+      </c>
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
       <c r="I40" s="22"/>
       <c r="J40" s="22"/>
       <c r="K40" s="22"/>
-      <c r="L40" s="28"/>
+      <c r="L40" s="27"/>
       <c r="M40" s="25"/>
       <c r="N40" s="17"/>
       <c r="O40" s="11"/>
@@ -3070,21 +3355,27 @@
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
     </row>
-    <row r="41" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A41" s="39"/>
-      <c r="B41" s="40"/>
+    <row r="41" spans="1:33" ht="39.6">
+      <c r="A41" s="61"/>
+      <c r="B41" s="61" t="s">
+        <v>68</v>
+      </c>
       <c r="C41" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="41"/>
+        <v>50</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>118</v>
+      </c>
       <c r="E41" s="26"/>
-      <c r="F41" s="24"/>
+      <c r="F41" s="24" t="s">
+        <v>165</v>
+      </c>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
       <c r="I41" s="22"/>
       <c r="J41" s="22"/>
       <c r="K41" s="22"/>
-      <c r="L41" s="28"/>
+      <c r="L41" s="27"/>
       <c r="M41" s="25"/>
       <c r="N41" s="17"/>
       <c r="O41" s="11"/>
@@ -3108,32 +3399,28 @@
       <c r="AG41" s="1"/>
     </row>
     <row r="42" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A42" s="39"/>
-      <c r="B42" s="38" t="s">
-        <v>108</v>
-      </c>
+      <c r="A42" s="61"/>
+      <c r="B42" s="61"/>
       <c r="C42" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
+        <v>82</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="26"/>
+      <c r="F42" s="24" t="s">
+        <v>166</v>
+      </c>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
       <c r="I42" s="22"/>
       <c r="J42" s="22"/>
       <c r="K42" s="22"/>
-      <c r="L42" s="28"/>
+      <c r="L42" s="27"/>
       <c r="M42" s="25"/>
-      <c r="N42" s="17">
-        <v>3</v>
-      </c>
-      <c r="O42" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P42" s="10"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
@@ -3153,30 +3440,28 @@
       <c r="AG42" s="1"/>
     </row>
     <row r="43" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
+      <c r="A43" s="61"/>
+      <c r="B43" s="61"/>
       <c r="C43" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
+        <v>83</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="26"/>
+      <c r="F43" s="24" t="s">
+        <v>165</v>
+      </c>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
       <c r="I43" s="22"/>
       <c r="J43" s="22"/>
       <c r="K43" s="22"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="17">
-        <v>3</v>
-      </c>
-      <c r="O43" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="P43" s="14"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
@@ -3196,30 +3481,28 @@
       <c r="AG43" s="1"/>
     </row>
     <row r="44" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="61"/>
+      <c r="B44" s="61"/>
       <c r="C44" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="D44" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
+        <v>84</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" s="26"/>
+      <c r="F44" s="24" t="s">
+        <v>142</v>
+      </c>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
       <c r="J44" s="22"/>
       <c r="K44" s="22"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="17">
-        <v>3</v>
-      </c>
-      <c r="O44" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="P44" s="15"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
@@ -3239,32 +3522,34 @@
       <c r="AG44" s="1"/>
     </row>
     <row r="45" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A45" s="39"/>
-      <c r="B45" s="38" t="s">
-        <v>109</v>
+      <c r="A45" s="61"/>
+      <c r="B45" s="61" t="s">
+        <v>125</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="30" t="s">
         <v>126</v>
       </c>
       <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
+      <c r="F45" s="20" t="s">
+        <v>147</v>
+      </c>
       <c r="G45" s="22"/>
       <c r="H45" s="22"/>
       <c r="I45" s="22"/>
       <c r="J45" s="22"/>
       <c r="K45" s="22"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="24"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="25"/>
       <c r="N45" s="17">
         <v>3</v>
       </c>
-      <c r="O45" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P45" s="15"/>
+      <c r="O45" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="P45" s="10"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
@@ -3284,28 +3569,32 @@
       <c r="AG45" s="1"/>
     </row>
     <row r="46" spans="1:33" ht="28.95" customHeight="1">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="65" t="s">
-        <v>127</v>
+      <c r="A46" s="61"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>135</v>
       </c>
       <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
+      <c r="F46" s="20" t="s">
+        <v>162</v>
+      </c>
       <c r="G46" s="22"/>
       <c r="H46" s="22"/>
       <c r="I46" s="22"/>
       <c r="J46" s="22"/>
       <c r="K46" s="22"/>
-      <c r="L46" s="28"/>
+      <c r="L46" s="27"/>
       <c r="M46" s="24"/>
       <c r="N46" s="17">
         <v>3</v>
       </c>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
+      <c r="O46" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P46" s="14"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
@@ -3324,17 +3613,33 @@
       <c r="AF46" s="1"/>
       <c r="AG46" s="1"/>
     </row>
-    <row r="47" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
+    <row r="47" spans="1:33" ht="28.95" customHeight="1">
+      <c r="A47" s="61"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="17">
+        <v>3</v>
+      </c>
+      <c r="O47" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="P47" s="15"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
@@ -3353,17 +3658,35 @@
       <c r="AF47" s="1"/>
       <c r="AG47" s="1"/>
     </row>
-    <row r="48" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
+    <row r="48" spans="1:33" ht="28.95" customHeight="1">
+      <c r="A48" s="61"/>
+      <c r="B48" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="24"/>
+      <c r="N48" s="17">
+        <v>3</v>
+      </c>
+      <c r="O48" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="P48" s="15"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
@@ -3382,20 +3705,29 @@
       <c r="AF48" s="1"/>
       <c r="AG48" s="1"/>
     </row>
-    <row r="49" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
+    <row r="49" spans="1:33" ht="28.95" customHeight="1">
+      <c r="A49" s="61"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="13"/>
+      <c r="P49" s="15"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
@@ -3414,23 +3746,31 @@
       <c r="AF49" s="1"/>
       <c r="AG49" s="1"/>
     </row>
-    <row r="50" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A50" s="1"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
+    <row r="50" spans="1:33" ht="28.95" customHeight="1">
+      <c r="A50" s="61"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="17">
+        <v>3</v>
+      </c>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
@@ -3449,21 +3789,31 @@
       <c r="AF50" s="1"/>
       <c r="AG50" s="1"/>
     </row>
-    <row r="51" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
+    <row r="51" spans="1:33" ht="39.6">
+      <c r="A51" s="61"/>
+      <c r="B51" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="27"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="59"/>
+      <c r="O51" s="60"/>
+      <c r="P51" s="60"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -3485,19 +3835,11 @@
     <row r="52" spans="1:33" ht="15.75" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K52" s="1"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="M52" s="2"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -3522,19 +3864,11 @@
     <row r="53" spans="1:33" ht="15.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K53" s="1"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="M53" s="2"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -3566,11 +3900,6 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K54" s="1"/>
-      <c r="L54" s="2"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -3603,11 +3932,9 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K55" s="1"/>
-      <c r="L55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
@@ -3640,11 +3967,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K56" s="1"/>
-      <c r="L56" s="2"/>
+      <c r="L56" s="16"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -3677,9 +4000,11 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="1"/>
+      <c r="J57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1"/>
+      <c r="L57" s="2"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
@@ -3712,9 +4037,11 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="1"/>
+      <c r="J58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K58" s="1"/>
+      <c r="L58" s="2"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -3747,9 +4074,11 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="1"/>
+      <c r="J59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K59" s="1"/>
+      <c r="L59" s="2"/>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
@@ -3782,9 +4111,11 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="1"/>
+      <c r="J60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K60" s="1"/>
+      <c r="L60" s="2"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
@@ -3817,9 +4148,11 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="1"/>
+      <c r="J61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K61" s="1"/>
+      <c r="L61" s="2"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
@@ -10387,11 +10720,181 @@
       <c r="AF248" s="1"/>
       <c r="AG248" s="1"/>
     </row>
-    <row r="249" spans="1:33" ht="15.75" customHeight="1"/>
-    <row r="250" spans="1:33" ht="15.75" customHeight="1"/>
-    <row r="251" spans="1:33" ht="15.75" customHeight="1"/>
-    <row r="252" spans="1:33" ht="15.75" customHeight="1"/>
-    <row r="253" spans="1:33" ht="15.75" customHeight="1"/>
+    <row r="249" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A249" s="1"/>
+      <c r="B249" s="2"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="1"/>
+      <c r="E249" s="2"/>
+      <c r="F249" s="2"/>
+      <c r="G249" s="2"/>
+      <c r="H249" s="2"/>
+      <c r="I249" s="2"/>
+      <c r="J249" s="2"/>
+      <c r="K249" s="2"/>
+      <c r="L249" s="1"/>
+      <c r="M249" s="1"/>
+      <c r="N249" s="1"/>
+      <c r="O249" s="1"/>
+      <c r="P249" s="1"/>
+      <c r="Q249" s="1"/>
+      <c r="R249" s="1"/>
+      <c r="S249" s="1"/>
+      <c r="T249" s="1"/>
+      <c r="U249" s="1"/>
+      <c r="V249" s="1"/>
+      <c r="W249" s="1"/>
+      <c r="X249" s="1"/>
+      <c r="Y249" s="1"/>
+      <c r="Z249" s="1"/>
+      <c r="AA249" s="1"/>
+      <c r="AB249" s="1"/>
+      <c r="AC249" s="1"/>
+      <c r="AD249" s="1"/>
+      <c r="AE249" s="1"/>
+      <c r="AF249" s="1"/>
+      <c r="AG249" s="1"/>
+    </row>
+    <row r="250" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A250" s="1"/>
+      <c r="B250" s="2"/>
+      <c r="C250" s="1"/>
+      <c r="D250" s="1"/>
+      <c r="E250" s="2"/>
+      <c r="F250" s="2"/>
+      <c r="G250" s="2"/>
+      <c r="H250" s="2"/>
+      <c r="I250" s="2"/>
+      <c r="J250" s="2"/>
+      <c r="K250" s="2"/>
+      <c r="L250" s="1"/>
+      <c r="M250" s="1"/>
+      <c r="N250" s="1"/>
+      <c r="O250" s="1"/>
+      <c r="P250" s="1"/>
+      <c r="Q250" s="1"/>
+      <c r="R250" s="1"/>
+      <c r="S250" s="1"/>
+      <c r="T250" s="1"/>
+      <c r="U250" s="1"/>
+      <c r="V250" s="1"/>
+      <c r="W250" s="1"/>
+      <c r="X250" s="1"/>
+      <c r="Y250" s="1"/>
+      <c r="Z250" s="1"/>
+      <c r="AA250" s="1"/>
+      <c r="AB250" s="1"/>
+      <c r="AC250" s="1"/>
+      <c r="AD250" s="1"/>
+      <c r="AE250" s="1"/>
+      <c r="AF250" s="1"/>
+      <c r="AG250" s="1"/>
+    </row>
+    <row r="251" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A251" s="1"/>
+      <c r="B251" s="2"/>
+      <c r="C251" s="1"/>
+      <c r="D251" s="1"/>
+      <c r="E251" s="2"/>
+      <c r="F251" s="2"/>
+      <c r="G251" s="2"/>
+      <c r="H251" s="2"/>
+      <c r="I251" s="2"/>
+      <c r="J251" s="2"/>
+      <c r="K251" s="2"/>
+      <c r="L251" s="1"/>
+      <c r="M251" s="1"/>
+      <c r="N251" s="1"/>
+      <c r="O251" s="1"/>
+      <c r="P251" s="1"/>
+      <c r="Q251" s="1"/>
+      <c r="R251" s="1"/>
+      <c r="S251" s="1"/>
+      <c r="T251" s="1"/>
+      <c r="U251" s="1"/>
+      <c r="V251" s="1"/>
+      <c r="W251" s="1"/>
+      <c r="X251" s="1"/>
+      <c r="Y251" s="1"/>
+      <c r="Z251" s="1"/>
+      <c r="AA251" s="1"/>
+      <c r="AB251" s="1"/>
+      <c r="AC251" s="1"/>
+      <c r="AD251" s="1"/>
+      <c r="AE251" s="1"/>
+      <c r="AF251" s="1"/>
+      <c r="AG251" s="1"/>
+    </row>
+    <row r="252" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A252" s="1"/>
+      <c r="B252" s="2"/>
+      <c r="C252" s="1"/>
+      <c r="D252" s="1"/>
+      <c r="E252" s="2"/>
+      <c r="F252" s="2"/>
+      <c r="G252" s="2"/>
+      <c r="H252" s="2"/>
+      <c r="I252" s="2"/>
+      <c r="J252" s="2"/>
+      <c r="K252" s="2"/>
+      <c r="L252" s="1"/>
+      <c r="M252" s="1"/>
+      <c r="N252" s="1"/>
+      <c r="O252" s="1"/>
+      <c r="P252" s="1"/>
+      <c r="Q252" s="1"/>
+      <c r="R252" s="1"/>
+      <c r="S252" s="1"/>
+      <c r="T252" s="1"/>
+      <c r="U252" s="1"/>
+      <c r="V252" s="1"/>
+      <c r="W252" s="1"/>
+      <c r="X252" s="1"/>
+      <c r="Y252" s="1"/>
+      <c r="Z252" s="1"/>
+      <c r="AA252" s="1"/>
+      <c r="AB252" s="1"/>
+      <c r="AC252" s="1"/>
+      <c r="AD252" s="1"/>
+      <c r="AE252" s="1"/>
+      <c r="AF252" s="1"/>
+      <c r="AG252" s="1"/>
+    </row>
+    <row r="253" spans="1:33" ht="15.75" customHeight="1">
+      <c r="A253" s="1"/>
+      <c r="B253" s="2"/>
+      <c r="C253" s="1"/>
+      <c r="D253" s="1"/>
+      <c r="E253" s="2"/>
+      <c r="F253" s="2"/>
+      <c r="G253" s="2"/>
+      <c r="H253" s="2"/>
+      <c r="I253" s="2"/>
+      <c r="J253" s="2"/>
+      <c r="K253" s="2"/>
+      <c r="L253" s="1"/>
+      <c r="M253" s="1"/>
+      <c r="N253" s="1"/>
+      <c r="O253" s="1"/>
+      <c r="P253" s="1"/>
+      <c r="Q253" s="1"/>
+      <c r="R253" s="1"/>
+      <c r="S253" s="1"/>
+      <c r="T253" s="1"/>
+      <c r="U253" s="1"/>
+      <c r="V253" s="1"/>
+      <c r="W253" s="1"/>
+      <c r="X253" s="1"/>
+      <c r="Y253" s="1"/>
+      <c r="Z253" s="1"/>
+      <c r="AA253" s="1"/>
+      <c r="AB253" s="1"/>
+      <c r="AC253" s="1"/>
+      <c r="AD253" s="1"/>
+      <c r="AE253" s="1"/>
+      <c r="AF253" s="1"/>
+      <c r="AG253" s="1"/>
+    </row>
     <row r="254" spans="1:33" ht="15.75" customHeight="1"/>
     <row r="255" spans="1:33" ht="15.75" customHeight="1"/>
     <row r="256" spans="1:33" ht="15.75" customHeight="1"/>
@@ -11148,32 +11651,37 @@
     <row r="1007" ht="15.75" customHeight="1"/>
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A7:P46" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A7:P50"/>
   <mergeCells count="14">
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A36:A46"/>
-    <mergeCell ref="A9:A35"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B38:B41"/>
     <mergeCell ref="B2:O3"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B19:B24"/>
     <mergeCell ref="B13:B18"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A38:A51"/>
+    <mergeCell ref="A9:A37"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="B35:B37"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -12209,7 +12717,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>